<commit_message>
Add postprocessing to the ability powers
</commit_message>
<xml_diff>
--- a/scripts/cards.xlsx
+++ b/scripts/cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\navarog\projects\wyrmsearch\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7257C1DD-0B3E-4056-AF3A-8766EB2C8137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{702BFF11-A14F-4E06-9AAC-5622663DDB88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Master" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="379">
   <si>
     <t>type</t>
   </si>
@@ -397,9 +397,6 @@
   </si>
   <si>
     <t>If you have at least as many dragons in your Golden Grotto as your left neighbor, gain [DragonCard].</t>
-  </si>
-  <si>
-    <t>Adventurer.</t>
   </si>
   <si>
     <t>Spry Horned Lung Dragon</t>
@@ -1533,19 +1530,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="85" workbookViewId="0">
+      <selection activeCell="E104" sqref="E104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" customWidth="1"/>
-    <col min="20" max="20" width="9.88671875" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="20" max="20" width="9.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1601,9 +1598,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1636,9 +1633,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1671,9 +1668,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1709,9 +1706,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1744,9 +1741,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1779,9 +1776,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1814,9 +1811,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1849,9 +1846,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1860,7 +1857,7 @@
         <v>39</v>
       </c>
       <c r="D9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -1884,9 +1881,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1922,9 +1919,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1960,9 +1957,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1995,9 +1992,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -2030,9 +2027,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -2065,9 +2062,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -2100,9 +2097,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -2135,9 +2132,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -2173,9 +2170,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -2211,9 +2208,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -2246,9 +2243,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -2284,9 +2281,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -2319,9 +2316,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -2354,9 +2351,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -2389,9 +2386,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -2424,9 +2421,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -2459,9 +2456,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -2494,9 +2491,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -2529,9 +2526,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -2564,9 +2561,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -2599,9 +2596,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -2634,9 +2631,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -2669,9 +2666,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -2704,9 +2701,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -2739,9 +2736,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -2774,9 +2771,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -2809,9 +2806,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -2844,9 +2841,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -2879,9 +2876,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -2914,9 +2911,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -2955,9 +2952,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -3002,9 +2999,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -3040,9 +3037,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -3081,9 +3078,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B43">
         <v>42</v>
@@ -3119,9 +3116,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B44">
         <v>43</v>
@@ -3154,9 +3151,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -3192,9 +3189,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B46">
         <v>45</v>
@@ -3227,9 +3224,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B47">
         <v>46</v>
@@ -3237,8 +3234,11 @@
       <c r="C47" t="s">
         <v>120</v>
       </c>
+      <c r="D47" t="s">
+        <v>121</v>
+      </c>
       <c r="E47" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="F47">
         <v>5</v>
@@ -3265,9 +3265,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B48">
         <v>47</v>
@@ -3279,7 +3279,7 @@
         <v>123</v>
       </c>
       <c r="E48" t="s">
-        <v>124</v>
+        <v>29</v>
       </c>
       <c r="F48">
         <v>5</v>
@@ -3300,18 +3300,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
       <c r="C49" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" t="s">
         <v>125</v>
-      </c>
-      <c r="D49" t="s">
-        <v>126</v>
       </c>
       <c r="E49" t="s">
         <v>16</v>
@@ -3335,18 +3335,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
       <c r="C50" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D50" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E50" t="s">
         <v>106</v>
@@ -3385,18 +3385,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
       <c r="C51" t="s">
+        <v>127</v>
+      </c>
+      <c r="D51" t="s">
         <v>128</v>
-      </c>
-      <c r="D51" t="s">
-        <v>129</v>
       </c>
       <c r="E51" t="s">
         <v>29</v>
@@ -3420,18 +3420,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B52">
         <v>51</v>
       </c>
       <c r="C52" t="s">
+        <v>129</v>
+      </c>
+      <c r="D52" t="s">
         <v>130</v>
-      </c>
-      <c r="D52" t="s">
-        <v>131</v>
       </c>
       <c r="E52" t="s">
         <v>106</v>
@@ -3461,18 +3461,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B53">
         <v>52</v>
       </c>
       <c r="C53" t="s">
+        <v>131</v>
+      </c>
+      <c r="D53" t="s">
         <v>132</v>
-      </c>
-      <c r="D53" t="s">
-        <v>133</v>
       </c>
       <c r="E53" t="s">
         <v>106</v>
@@ -3499,18 +3499,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B54">
         <v>53</v>
       </c>
       <c r="C54" t="s">
+        <v>133</v>
+      </c>
+      <c r="D54" t="s">
         <v>134</v>
-      </c>
-      <c r="D54" t="s">
-        <v>135</v>
       </c>
       <c r="E54" t="s">
         <v>29</v>
@@ -3537,18 +3537,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B55">
         <v>54</v>
       </c>
       <c r="C55" t="s">
+        <v>135</v>
+      </c>
+      <c r="D55" t="s">
         <v>136</v>
-      </c>
-      <c r="D55" t="s">
-        <v>137</v>
       </c>
       <c r="E55" t="s">
         <v>106</v>
@@ -3584,18 +3584,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B56">
         <v>55</v>
       </c>
       <c r="C56" t="s">
+        <v>137</v>
+      </c>
+      <c r="D56" t="s">
         <v>138</v>
-      </c>
-      <c r="D56" t="s">
-        <v>139</v>
       </c>
       <c r="E56" t="s">
         <v>29</v>
@@ -3625,18 +3625,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B57">
         <v>56</v>
       </c>
       <c r="C57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D57" t="s">
         <v>140</v>
-      </c>
-      <c r="D57" t="s">
-        <v>141</v>
       </c>
       <c r="E57" t="s">
         <v>29</v>
@@ -3666,18 +3666,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B58">
         <v>57</v>
       </c>
       <c r="C58" t="s">
+        <v>141</v>
+      </c>
+      <c r="D58" t="s">
         <v>142</v>
-      </c>
-      <c r="D58" t="s">
-        <v>143</v>
       </c>
       <c r="E58" t="s">
         <v>16</v>
@@ -3704,18 +3704,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B59">
         <v>58</v>
       </c>
       <c r="C59" t="s">
+        <v>143</v>
+      </c>
+      <c r="D59" t="s">
         <v>144</v>
-      </c>
-      <c r="D59" t="s">
-        <v>145</v>
       </c>
       <c r="E59" t="s">
         <v>29</v>
@@ -3742,18 +3742,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B60">
         <v>59</v>
       </c>
       <c r="C60" t="s">
+        <v>146</v>
+      </c>
+      <c r="D60" t="s">
         <v>147</v>
-      </c>
-      <c r="D60" t="s">
-        <v>148</v>
       </c>
       <c r="E60" t="s">
         <v>106</v>
@@ -3783,18 +3783,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B61">
         <v>60</v>
       </c>
       <c r="C61" t="s">
+        <v>148</v>
+      </c>
+      <c r="D61" t="s">
         <v>149</v>
-      </c>
-      <c r="D61" t="s">
-        <v>150</v>
       </c>
       <c r="E61" t="s">
         <v>16</v>
@@ -3821,18 +3821,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
       <c r="C62" t="s">
+        <v>150</v>
+      </c>
+      <c r="D62" t="s">
         <v>151</v>
-      </c>
-      <c r="D62" t="s">
-        <v>152</v>
       </c>
       <c r="E62" t="s">
         <v>29</v>
@@ -3865,18 +3865,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B63">
         <v>62</v>
       </c>
       <c r="C63" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D63" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E63" t="s">
         <v>16</v>
@@ -3900,21 +3900,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B64">
         <v>63</v>
       </c>
       <c r="C64" t="s">
+        <v>153</v>
+      </c>
+      <c r="D64" t="s">
         <v>154</v>
       </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>155</v>
-      </c>
-      <c r="E64" t="s">
-        <v>156</v>
       </c>
       <c r="F64">
         <v>6</v>
@@ -3944,18 +3944,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B65">
         <v>64</v>
       </c>
       <c r="C65" t="s">
+        <v>156</v>
+      </c>
+      <c r="D65" t="s">
         <v>157</v>
-      </c>
-      <c r="D65" t="s">
-        <v>158</v>
       </c>
       <c r="E65" t="s">
         <v>16</v>
@@ -3979,18 +3979,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B66">
         <v>65</v>
       </c>
       <c r="C66" t="s">
+        <v>158</v>
+      </c>
+      <c r="D66" t="s">
         <v>159</v>
-      </c>
-      <c r="D66" t="s">
-        <v>160</v>
       </c>
       <c r="E66" t="s">
         <v>16</v>
@@ -4017,18 +4017,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B67">
         <v>66</v>
       </c>
       <c r="C67" t="s">
+        <v>160</v>
+      </c>
+      <c r="D67" t="s">
         <v>161</v>
-      </c>
-      <c r="D67" t="s">
-        <v>162</v>
       </c>
       <c r="E67" t="s">
         <v>29</v>
@@ -4055,18 +4055,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B68">
         <v>67</v>
       </c>
       <c r="C68" t="s">
+        <v>162</v>
+      </c>
+      <c r="D68" t="s">
         <v>163</v>
-      </c>
-      <c r="D68" t="s">
-        <v>164</v>
       </c>
       <c r="E68" t="s">
         <v>29</v>
@@ -4096,18 +4096,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B69">
         <v>68</v>
       </c>
       <c r="C69" t="s">
+        <v>164</v>
+      </c>
+      <c r="D69" t="s">
         <v>165</v>
-      </c>
-      <c r="D69" t="s">
-        <v>166</v>
       </c>
       <c r="E69" t="s">
         <v>29</v>
@@ -4131,21 +4131,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B70">
         <v>69</v>
       </c>
       <c r="C70" t="s">
+        <v>166</v>
+      </c>
+      <c r="D70" t="s">
         <v>167</v>
       </c>
-      <c r="D70" t="s">
-        <v>168</v>
-      </c>
       <c r="E70" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F70">
         <v>3</v>
@@ -4166,21 +4166,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B71">
         <v>70</v>
       </c>
       <c r="C71" t="s">
+        <v>168</v>
+      </c>
+      <c r="D71" t="s">
         <v>169</v>
       </c>
-      <c r="D71" t="s">
-        <v>170</v>
-      </c>
       <c r="E71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F71">
         <v>5</v>
@@ -4207,18 +4207,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B72">
         <v>71</v>
       </c>
       <c r="C72" t="s">
+        <v>170</v>
+      </c>
+      <c r="D72" t="s">
         <v>171</v>
-      </c>
-      <c r="D72" t="s">
-        <v>172</v>
       </c>
       <c r="E72" t="s">
         <v>106</v>
@@ -4248,21 +4248,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B73">
         <v>72</v>
       </c>
       <c r="C73" t="s">
+        <v>172</v>
+      </c>
+      <c r="D73" t="s">
         <v>173</v>
       </c>
-      <c r="D73" t="s">
-        <v>174</v>
-      </c>
       <c r="E73" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F73">
         <v>5</v>
@@ -4286,18 +4286,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B74">
         <v>73</v>
       </c>
       <c r="C74" t="s">
+        <v>174</v>
+      </c>
+      <c r="D74" t="s">
         <v>175</v>
-      </c>
-      <c r="D74" t="s">
-        <v>176</v>
       </c>
       <c r="E74" t="s">
         <v>29</v>
@@ -4324,18 +4324,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B75">
         <v>74</v>
       </c>
       <c r="C75" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D75" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E75" t="s">
         <v>106</v>
@@ -4362,18 +4362,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B76">
         <v>75</v>
       </c>
       <c r="C76" t="s">
+        <v>178</v>
+      </c>
+      <c r="D76" t="s">
         <v>179</v>
-      </c>
-      <c r="D76" t="s">
-        <v>180</v>
       </c>
       <c r="E76" t="s">
         <v>29</v>
@@ -4400,18 +4400,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B77">
         <v>76</v>
       </c>
       <c r="C77" t="s">
+        <v>180</v>
+      </c>
+      <c r="D77" t="s">
         <v>181</v>
-      </c>
-      <c r="D77" t="s">
-        <v>182</v>
       </c>
       <c r="E77" t="s">
         <v>16</v>
@@ -4438,18 +4438,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B78">
         <v>77</v>
       </c>
       <c r="C78" t="s">
+        <v>182</v>
+      </c>
+      <c r="D78" t="s">
         <v>183</v>
-      </c>
-      <c r="D78" t="s">
-        <v>184</v>
       </c>
       <c r="E78" t="s">
         <v>29</v>
@@ -4479,18 +4479,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B79">
         <v>78</v>
       </c>
       <c r="C79" t="s">
+        <v>184</v>
+      </c>
+      <c r="D79" t="s">
         <v>185</v>
-      </c>
-      <c r="D79" t="s">
-        <v>186</v>
       </c>
       <c r="E79" t="s">
         <v>29</v>
@@ -4514,21 +4514,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B80">
         <v>79</v>
       </c>
       <c r="C80" t="s">
+        <v>186</v>
+      </c>
+      <c r="D80" t="s">
         <v>187</v>
       </c>
-      <c r="D80" t="s">
-        <v>188</v>
-      </c>
       <c r="E80" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -4552,18 +4552,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B81">
         <v>80</v>
       </c>
       <c r="C81" t="s">
+        <v>188</v>
+      </c>
+      <c r="D81" t="s">
         <v>189</v>
-      </c>
-      <c r="D81" t="s">
-        <v>190</v>
       </c>
       <c r="E81" t="s">
         <v>29</v>
@@ -4593,18 +4593,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B82">
         <v>81</v>
       </c>
       <c r="C82" t="s">
+        <v>190</v>
+      </c>
+      <c r="D82" t="s">
         <v>191</v>
-      </c>
-      <c r="D82" t="s">
-        <v>192</v>
       </c>
       <c r="E82" t="s">
         <v>106</v>
@@ -4631,18 +4631,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B83">
         <v>82</v>
       </c>
       <c r="C83" t="s">
+        <v>192</v>
+      </c>
+      <c r="D83" t="s">
         <v>193</v>
-      </c>
-      <c r="D83" t="s">
-        <v>194</v>
       </c>
       <c r="E83" t="s">
         <v>29</v>
@@ -4666,18 +4666,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B84">
         <v>83</v>
       </c>
       <c r="C84" t="s">
+        <v>194</v>
+      </c>
+      <c r="D84" t="s">
         <v>195</v>
-      </c>
-      <c r="D84" t="s">
-        <v>196</v>
       </c>
       <c r="E84" t="s">
         <v>16</v>
@@ -4704,18 +4704,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B85">
         <v>84</v>
       </c>
       <c r="C85" t="s">
+        <v>196</v>
+      </c>
+      <c r="D85" t="s">
         <v>197</v>
-      </c>
-      <c r="D85" t="s">
-        <v>198</v>
       </c>
       <c r="E85" t="s">
         <v>29</v>
@@ -4742,18 +4742,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B86">
         <v>85</v>
       </c>
       <c r="C86" t="s">
+        <v>198</v>
+      </c>
+      <c r="D86" t="s">
         <v>199</v>
-      </c>
-      <c r="D86" t="s">
-        <v>200</v>
       </c>
       <c r="E86" t="s">
         <v>16</v>
@@ -4780,18 +4780,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B87">
         <v>86</v>
       </c>
       <c r="C87" t="s">
+        <v>200</v>
+      </c>
+      <c r="D87" t="s">
         <v>201</v>
-      </c>
-      <c r="D87" t="s">
-        <v>202</v>
       </c>
       <c r="E87" t="s">
         <v>106</v>
@@ -4818,18 +4818,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B88">
         <v>87</v>
       </c>
       <c r="C88" t="s">
+        <v>202</v>
+      </c>
+      <c r="D88" t="s">
         <v>203</v>
-      </c>
-      <c r="D88" t="s">
-        <v>204</v>
       </c>
       <c r="E88" t="s">
         <v>106</v>
@@ -4859,18 +4859,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B89">
         <v>88</v>
       </c>
       <c r="C89" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D89" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E89" t="s">
         <v>16</v>
@@ -4894,18 +4894,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B90">
         <v>89</v>
       </c>
       <c r="C90" t="s">
+        <v>205</v>
+      </c>
+      <c r="D90" t="s">
         <v>206</v>
-      </c>
-      <c r="D90" t="s">
-        <v>207</v>
       </c>
       <c r="E90" t="s">
         <v>16</v>
@@ -4935,18 +4935,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B91">
         <v>90</v>
       </c>
       <c r="C91" t="s">
+        <v>207</v>
+      </c>
+      <c r="D91" t="s">
         <v>208</v>
-      </c>
-      <c r="D91" t="s">
-        <v>209</v>
       </c>
       <c r="E91" t="s">
         <v>29</v>
@@ -4976,18 +4976,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B92">
         <v>91</v>
       </c>
       <c r="C92" t="s">
+        <v>209</v>
+      </c>
+      <c r="D92" t="s">
         <v>210</v>
-      </c>
-      <c r="D92" t="s">
-        <v>211</v>
       </c>
       <c r="E92" t="s">
         <v>106</v>
@@ -5023,18 +5023,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B93">
         <v>92</v>
       </c>
       <c r="C93" t="s">
+        <v>211</v>
+      </c>
+      <c r="D93" t="s">
         <v>212</v>
-      </c>
-      <c r="D93" t="s">
-        <v>213</v>
       </c>
       <c r="E93" t="s">
         <v>29</v>
@@ -5058,18 +5058,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B94">
         <v>93</v>
       </c>
       <c r="C94" t="s">
+        <v>213</v>
+      </c>
+      <c r="D94" t="s">
         <v>214</v>
-      </c>
-      <c r="D94" t="s">
-        <v>215</v>
       </c>
       <c r="E94" t="s">
         <v>106</v>
@@ -5093,18 +5093,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B95">
         <v>94</v>
       </c>
       <c r="C95" t="s">
+        <v>215</v>
+      </c>
+      <c r="D95" t="s">
         <v>216</v>
-      </c>
-      <c r="D95" t="s">
-        <v>217</v>
       </c>
       <c r="E95" t="s">
         <v>29</v>
@@ -5134,21 +5134,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B96">
         <v>95</v>
       </c>
       <c r="C96" t="s">
+        <v>217</v>
+      </c>
+      <c r="D96" t="s">
         <v>218</v>
       </c>
-      <c r="D96" t="s">
-        <v>219</v>
-      </c>
       <c r="E96" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F96">
         <v>3</v>
@@ -5175,18 +5175,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B97">
         <v>96</v>
       </c>
       <c r="C97" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D97" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="E97" t="s">
         <v>29</v>
@@ -5216,18 +5216,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B98">
         <v>97</v>
       </c>
       <c r="C98" t="s">
+        <v>220</v>
+      </c>
+      <c r="D98" t="s">
         <v>221</v>
-      </c>
-      <c r="D98" t="s">
-        <v>222</v>
       </c>
       <c r="E98" t="s">
         <v>106</v>
@@ -5260,18 +5260,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B99">
         <v>98</v>
       </c>
       <c r="C99" t="s">
+        <v>222</v>
+      </c>
+      <c r="D99" t="s">
         <v>223</v>
-      </c>
-      <c r="D99" t="s">
-        <v>224</v>
       </c>
       <c r="E99" t="s">
         <v>106</v>
@@ -5295,18 +5295,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B100">
         <v>99</v>
       </c>
       <c r="C100" t="s">
+        <v>224</v>
+      </c>
+      <c r="D100" t="s">
         <v>225</v>
-      </c>
-      <c r="D100" t="s">
-        <v>226</v>
       </c>
       <c r="E100" t="s">
         <v>16</v>
@@ -5336,18 +5336,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B101">
         <v>100</v>
       </c>
       <c r="C101" t="s">
+        <v>226</v>
+      </c>
+      <c r="D101" t="s">
         <v>227</v>
-      </c>
-      <c r="D101" t="s">
-        <v>228</v>
       </c>
       <c r="E101" t="s">
         <v>29</v>
@@ -5374,18 +5374,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B102">
         <v>101</v>
       </c>
       <c r="C102" t="s">
+        <v>228</v>
+      </c>
+      <c r="D102" t="s">
         <v>229</v>
-      </c>
-      <c r="D102" t="s">
-        <v>230</v>
       </c>
       <c r="E102" t="s">
         <v>106</v>
@@ -5424,18 +5424,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B103">
         <v>102</v>
       </c>
       <c r="C103" t="s">
+        <v>230</v>
+      </c>
+      <c r="D103" t="s">
         <v>231</v>
-      </c>
-      <c r="D103" t="s">
-        <v>232</v>
       </c>
       <c r="E103" t="s">
         <v>106</v>
@@ -5465,18 +5465,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B104">
         <v>103</v>
       </c>
       <c r="C104" t="s">
+        <v>232</v>
+      </c>
+      <c r="D104" t="s">
         <v>233</v>
       </c>
       <c r="E104" t="s">
-        <v>234</v>
+        <v>106</v>
       </c>
       <c r="F104">
         <v>3</v>
@@ -5497,21 +5500,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B105">
         <v>104</v>
       </c>
       <c r="C105" t="s">
+        <v>234</v>
+      </c>
+      <c r="D105" t="s">
         <v>235</v>
       </c>
-      <c r="D105" t="s">
-        <v>236</v>
-      </c>
       <c r="E105" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F105">
         <v>0</v>
@@ -5535,18 +5538,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B106">
         <v>105</v>
       </c>
       <c r="C106" t="s">
+        <v>236</v>
+      </c>
+      <c r="D106" t="s">
         <v>237</v>
-      </c>
-      <c r="D106" t="s">
-        <v>238</v>
       </c>
       <c r="E106" t="s">
         <v>16</v>
@@ -5570,18 +5573,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B107">
         <v>106</v>
       </c>
       <c r="C107" t="s">
+        <v>238</v>
+      </c>
+      <c r="D107" t="s">
         <v>239</v>
-      </c>
-      <c r="D107" t="s">
-        <v>240</v>
       </c>
       <c r="E107" t="s">
         <v>106</v>
@@ -5611,21 +5614,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B108">
         <v>107</v>
       </c>
       <c r="C108" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D108" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E108" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F108">
         <v>1</v>
@@ -5646,18 +5649,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B109">
         <v>108</v>
       </c>
       <c r="C109" t="s">
+        <v>241</v>
+      </c>
+      <c r="D109" t="s">
         <v>242</v>
-      </c>
-      <c r="D109" t="s">
-        <v>243</v>
       </c>
       <c r="E109" t="s">
         <v>16</v>
@@ -5684,21 +5687,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B110">
         <v>109</v>
       </c>
       <c r="C110" t="s">
+        <v>243</v>
+      </c>
+      <c r="D110" t="s">
         <v>244</v>
       </c>
-      <c r="D110" t="s">
-        <v>245</v>
-      </c>
       <c r="E110" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F110">
         <v>5</v>
@@ -5725,18 +5728,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B111">
         <v>110</v>
       </c>
       <c r="C111" t="s">
+        <v>245</v>
+      </c>
+      <c r="D111" t="s">
         <v>246</v>
-      </c>
-      <c r="D111" t="s">
-        <v>247</v>
       </c>
       <c r="E111" t="s">
         <v>29</v>
@@ -5760,21 +5763,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B112">
         <v>111</v>
       </c>
       <c r="C112" t="s">
+        <v>247</v>
+      </c>
+      <c r="D112" t="s">
         <v>248</v>
       </c>
-      <c r="D112" t="s">
-        <v>249</v>
-      </c>
       <c r="E112" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -5798,18 +5801,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B113">
         <v>112</v>
       </c>
       <c r="C113" t="s">
+        <v>249</v>
+      </c>
+      <c r="D113" t="s">
         <v>250</v>
-      </c>
-      <c r="D113" t="s">
-        <v>251</v>
       </c>
       <c r="E113" t="s">
         <v>106</v>
@@ -5845,18 +5848,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B114">
         <v>113</v>
       </c>
       <c r="C114" t="s">
+        <v>251</v>
+      </c>
+      <c r="D114" t="s">
         <v>252</v>
-      </c>
-      <c r="D114" t="s">
-        <v>253</v>
       </c>
       <c r="E114" t="s">
         <v>16</v>
@@ -5883,18 +5886,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B115">
         <v>114</v>
       </c>
       <c r="C115" t="s">
+        <v>253</v>
+      </c>
+      <c r="D115" t="s">
         <v>254</v>
-      </c>
-      <c r="D115" t="s">
-        <v>255</v>
       </c>
       <c r="E115" t="s">
         <v>29</v>
@@ -5918,18 +5921,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B116">
         <v>115</v>
       </c>
       <c r="C116" t="s">
+        <v>255</v>
+      </c>
+      <c r="D116" t="s">
         <v>256</v>
-      </c>
-      <c r="D116" t="s">
-        <v>257</v>
       </c>
       <c r="E116" t="s">
         <v>16</v>
@@ -5959,18 +5962,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B117">
         <v>116</v>
       </c>
       <c r="C117" t="s">
+        <v>257</v>
+      </c>
+      <c r="D117" t="s">
         <v>258</v>
-      </c>
-      <c r="D117" t="s">
-        <v>259</v>
       </c>
       <c r="E117" t="s">
         <v>16</v>
@@ -5997,21 +6000,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B118">
         <v>117</v>
       </c>
       <c r="C118" t="s">
+        <v>259</v>
+      </c>
+      <c r="D118" t="s">
         <v>260</v>
       </c>
-      <c r="D118" t="s">
-        <v>261</v>
-      </c>
       <c r="E118" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F118">
         <v>2</v>
@@ -6038,15 +6041,15 @@
         <v>24</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B119">
         <v>118</v>
       </c>
       <c r="C119" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D119" t="s">
         <v>102</v>
@@ -6079,18 +6082,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B120">
         <v>119</v>
       </c>
       <c r="C120" t="s">
+        <v>262</v>
+      </c>
+      <c r="D120" t="s">
         <v>263</v>
-      </c>
-      <c r="D120" t="s">
-        <v>264</v>
       </c>
       <c r="E120" t="s">
         <v>106</v>
@@ -6129,21 +6132,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B121">
         <v>120</v>
       </c>
       <c r="C121" t="s">
+        <v>264</v>
+      </c>
+      <c r="D121" t="s">
         <v>265</v>
       </c>
-      <c r="D121" t="s">
-        <v>266</v>
-      </c>
       <c r="E121" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F121">
         <v>4</v>
@@ -6170,18 +6173,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B122">
         <v>121</v>
       </c>
       <c r="C122" t="s">
+        <v>266</v>
+      </c>
+      <c r="D122" t="s">
         <v>267</v>
-      </c>
-      <c r="D122" t="s">
-        <v>268</v>
       </c>
       <c r="E122" t="s">
         <v>16</v>
@@ -6208,18 +6211,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B123">
         <v>122</v>
       </c>
       <c r="C123" t="s">
+        <v>268</v>
+      </c>
+      <c r="D123" t="s">
         <v>269</v>
-      </c>
-      <c r="D123" t="s">
-        <v>270</v>
       </c>
       <c r="E123" t="s">
         <v>106</v>
@@ -6246,18 +6249,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B124">
         <v>123</v>
       </c>
       <c r="C124" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D124" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E124" t="s">
         <v>29</v>
@@ -6287,18 +6290,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B125">
         <v>124</v>
       </c>
       <c r="C125" t="s">
+        <v>271</v>
+      </c>
+      <c r="D125" t="s">
         <v>272</v>
-      </c>
-      <c r="D125" t="s">
-        <v>273</v>
       </c>
       <c r="E125" t="s">
         <v>106</v>
@@ -6337,18 +6340,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B126">
         <v>125</v>
       </c>
       <c r="C126" t="s">
+        <v>273</v>
+      </c>
+      <c r="D126" t="s">
         <v>274</v>
-      </c>
-      <c r="D126" t="s">
-        <v>275</v>
       </c>
       <c r="E126" t="s">
         <v>29</v>
@@ -6372,18 +6375,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B127">
         <v>126</v>
       </c>
       <c r="C127" t="s">
+        <v>275</v>
+      </c>
+      <c r="D127" t="s">
         <v>276</v>
-      </c>
-      <c r="D127" t="s">
-        <v>277</v>
       </c>
       <c r="E127" t="s">
         <v>29</v>
@@ -6410,18 +6413,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B128">
         <v>127</v>
       </c>
       <c r="C128" t="s">
+        <v>277</v>
+      </c>
+      <c r="D128" t="s">
         <v>278</v>
-      </c>
-      <c r="D128" t="s">
-        <v>279</v>
       </c>
       <c r="E128" t="s">
         <v>29</v>
@@ -6445,18 +6448,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B129">
         <v>128</v>
       </c>
       <c r="C129" t="s">
+        <v>279</v>
+      </c>
+      <c r="D129" t="s">
         <v>280</v>
-      </c>
-      <c r="D129" t="s">
-        <v>281</v>
       </c>
       <c r="E129" t="s">
         <v>29</v>
@@ -6483,18 +6486,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B130">
         <v>129</v>
       </c>
       <c r="C130" t="s">
+        <v>281</v>
+      </c>
+      <c r="D130" t="s">
         <v>282</v>
-      </c>
-      <c r="D130" t="s">
-        <v>283</v>
       </c>
       <c r="E130" t="s">
         <v>106</v>
@@ -6527,21 +6530,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B131">
         <v>130</v>
       </c>
       <c r="C131" t="s">
+        <v>283</v>
+      </c>
+      <c r="D131" t="s">
         <v>284</v>
       </c>
-      <c r="D131" t="s">
-        <v>285</v>
-      </c>
       <c r="E131" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F131">
         <v>2</v>
@@ -6562,18 +6565,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B132">
         <v>131</v>
       </c>
       <c r="C132" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D132" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E132" t="s">
         <v>106</v>
@@ -6612,18 +6615,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B133">
         <v>132</v>
       </c>
       <c r="C133" t="s">
+        <v>287</v>
+      </c>
+      <c r="D133" t="s">
         <v>288</v>
-      </c>
-      <c r="D133" t="s">
-        <v>289</v>
       </c>
       <c r="E133" t="s">
         <v>106</v>
@@ -6662,18 +6665,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B134">
         <v>133</v>
       </c>
       <c r="C134" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D134" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E134" t="s">
         <v>29</v>
@@ -6703,18 +6706,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B135">
         <v>134</v>
       </c>
       <c r="C135" t="s">
+        <v>290</v>
+      </c>
+      <c r="D135" t="s">
         <v>291</v>
-      </c>
-      <c r="D135" t="s">
-        <v>292</v>
       </c>
       <c r="E135" t="s">
         <v>106</v>
@@ -6753,21 +6756,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B136">
         <v>135</v>
       </c>
       <c r="C136" t="s">
+        <v>292</v>
+      </c>
+      <c r="D136" t="s">
         <v>293</v>
       </c>
-      <c r="D136" t="s">
-        <v>294</v>
-      </c>
       <c r="E136" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F136">
         <v>2</v>
@@ -6794,18 +6797,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B137">
         <v>136</v>
       </c>
       <c r="C137" t="s">
+        <v>294</v>
+      </c>
+      <c r="D137" t="s">
         <v>295</v>
-      </c>
-      <c r="D137" t="s">
-        <v>296</v>
       </c>
       <c r="E137" t="s">
         <v>29</v>
@@ -6832,18 +6835,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B138">
         <v>137</v>
       </c>
       <c r="C138" t="s">
+        <v>296</v>
+      </c>
+      <c r="D138" t="s">
         <v>297</v>
-      </c>
-      <c r="D138" t="s">
-        <v>298</v>
       </c>
       <c r="E138" t="s">
         <v>29</v>
@@ -6870,21 +6873,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B139">
         <v>138</v>
       </c>
       <c r="C139" t="s">
+        <v>298</v>
+      </c>
+      <c r="D139" t="s">
         <v>299</v>
       </c>
-      <c r="D139" t="s">
-        <v>300</v>
-      </c>
       <c r="E139" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F139">
         <v>1</v>
@@ -6905,21 +6908,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B140">
         <v>139</v>
       </c>
       <c r="C140" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D140" t="s">
         <v>115</v>
       </c>
       <c r="E140" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F140">
         <v>4</v>
@@ -6946,18 +6949,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B141">
         <v>140</v>
       </c>
       <c r="C141" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D141" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E141" t="s">
         <v>16</v>
@@ -6984,21 +6987,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B142">
         <v>141</v>
       </c>
       <c r="C142" t="s">
+        <v>302</v>
+      </c>
+      <c r="D142" t="s">
         <v>303</v>
       </c>
-      <c r="D142" t="s">
-        <v>304</v>
-      </c>
       <c r="E142" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F142">
         <v>3</v>
@@ -7025,21 +7028,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B143">
         <v>142</v>
       </c>
       <c r="C143" t="s">
+        <v>304</v>
+      </c>
+      <c r="D143" t="s">
         <v>305</v>
       </c>
-      <c r="D143" t="s">
-        <v>306</v>
-      </c>
       <c r="E143" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F143">
         <v>3</v>
@@ -7066,18 +7069,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B144">
         <v>143</v>
       </c>
       <c r="C144" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D144" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E144" t="s">
         <v>29</v>
@@ -7104,18 +7107,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B145">
         <v>144</v>
       </c>
       <c r="C145" t="s">
+        <v>307</v>
+      </c>
+      <c r="D145" t="s">
         <v>308</v>
-      </c>
-      <c r="D145" t="s">
-        <v>309</v>
       </c>
       <c r="E145" t="s">
         <v>106</v>
@@ -7154,18 +7157,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B146">
         <v>145</v>
       </c>
       <c r="C146" t="s">
+        <v>309</v>
+      </c>
+      <c r="D146" t="s">
         <v>310</v>
-      </c>
-      <c r="D146" t="s">
-        <v>311</v>
       </c>
       <c r="E146" t="s">
         <v>106</v>
@@ -7189,18 +7192,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B147">
         <v>146</v>
       </c>
       <c r="C147" t="s">
+        <v>311</v>
+      </c>
+      <c r="D147" t="s">
         <v>312</v>
-      </c>
-      <c r="D147" t="s">
-        <v>313</v>
       </c>
       <c r="E147" t="s">
         <v>16</v>
@@ -7224,18 +7227,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B148">
         <v>147</v>
       </c>
       <c r="C148" t="s">
+        <v>313</v>
+      </c>
+      <c r="D148" t="s">
         <v>314</v>
-      </c>
-      <c r="D148" t="s">
-        <v>315</v>
       </c>
       <c r="E148" t="s">
         <v>16</v>
@@ -7262,18 +7265,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B149">
         <v>148</v>
       </c>
       <c r="C149" t="s">
+        <v>315</v>
+      </c>
+      <c r="D149" t="s">
         <v>316</v>
-      </c>
-      <c r="D149" t="s">
-        <v>317</v>
       </c>
       <c r="E149" t="s">
         <v>29</v>
@@ -7300,18 +7303,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B150">
         <v>149</v>
       </c>
       <c r="C150" t="s">
+        <v>317</v>
+      </c>
+      <c r="D150" t="s">
         <v>318</v>
-      </c>
-      <c r="D150" t="s">
-        <v>319</v>
       </c>
       <c r="E150" t="s">
         <v>106</v>
@@ -7347,18 +7350,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B151">
         <v>150</v>
       </c>
       <c r="C151" t="s">
+        <v>319</v>
+      </c>
+      <c r="D151" t="s">
         <v>320</v>
-      </c>
-      <c r="D151" t="s">
-        <v>321</v>
       </c>
       <c r="E151" t="s">
         <v>106</v>
@@ -7394,18 +7397,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B152">
         <v>151</v>
       </c>
       <c r="C152" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D152" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E152" t="s">
         <v>29</v>
@@ -7432,18 +7435,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B153">
         <v>152</v>
       </c>
       <c r="C153" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D153" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E153" t="s">
         <v>29</v>
@@ -7467,21 +7470,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B154">
         <v>153</v>
       </c>
       <c r="C154" t="s">
+        <v>323</v>
+      </c>
+      <c r="D154" t="s">
         <v>324</v>
       </c>
-      <c r="D154" t="s">
-        <v>325</v>
-      </c>
       <c r="E154" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F154">
         <v>2</v>
@@ -7508,21 +7511,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B155">
         <v>154</v>
       </c>
       <c r="C155" t="s">
+        <v>325</v>
+      </c>
+      <c r="D155" t="s">
         <v>326</v>
       </c>
-      <c r="D155" t="s">
-        <v>327</v>
-      </c>
       <c r="E155" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F155">
         <v>3</v>
@@ -7549,18 +7552,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B156">
         <v>155</v>
       </c>
       <c r="C156" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D156" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E156" t="s">
         <v>29</v>
@@ -7587,18 +7590,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B157">
         <v>156</v>
       </c>
       <c r="C157" t="s">
+        <v>328</v>
+      </c>
+      <c r="D157" t="s">
         <v>329</v>
-      </c>
-      <c r="D157" t="s">
-        <v>330</v>
       </c>
       <c r="E157" t="s">
         <v>16</v>
@@ -7622,18 +7625,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B158">
         <v>157</v>
       </c>
       <c r="C158" t="s">
+        <v>330</v>
+      </c>
+      <c r="D158" t="s">
         <v>331</v>
-      </c>
-      <c r="D158" t="s">
-        <v>332</v>
       </c>
       <c r="E158" t="s">
         <v>16</v>
@@ -7660,18 +7663,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B159">
         <v>158</v>
       </c>
       <c r="C159" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D159" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E159" t="s">
         <v>29</v>
@@ -7698,18 +7701,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B160">
         <v>159</v>
       </c>
       <c r="C160" t="s">
+        <v>333</v>
+      </c>
+      <c r="D160" t="s">
         <v>334</v>
-      </c>
-      <c r="D160" t="s">
-        <v>335</v>
       </c>
       <c r="E160" t="s">
         <v>29</v>
@@ -7736,21 +7739,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B161">
         <v>160</v>
       </c>
       <c r="C161" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D161" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E161" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F161">
         <v>3</v>
@@ -7771,21 +7774,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B162">
         <v>161</v>
       </c>
       <c r="C162" t="s">
+        <v>336</v>
+      </c>
+      <c r="D162" t="s">
         <v>337</v>
       </c>
-      <c r="D162" t="s">
-        <v>338</v>
-      </c>
       <c r="E162" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F162">
         <v>4</v>
@@ -7809,18 +7812,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B163">
         <v>162</v>
       </c>
       <c r="C163" t="s">
+        <v>338</v>
+      </c>
+      <c r="D163" t="s">
         <v>339</v>
-      </c>
-      <c r="D163" t="s">
-        <v>340</v>
       </c>
       <c r="E163" t="s">
         <v>16</v>
@@ -7847,18 +7850,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B164">
         <v>163</v>
       </c>
       <c r="C164" t="s">
+        <v>340</v>
+      </c>
+      <c r="D164" t="s">
         <v>341</v>
-      </c>
-      <c r="D164" t="s">
-        <v>342</v>
       </c>
       <c r="E164" t="s">
         <v>29</v>
@@ -7885,21 +7888,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B165">
         <v>164</v>
       </c>
       <c r="C165" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D165" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E165" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F165">
         <v>4</v>
@@ -7923,18 +7926,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B166">
         <v>165</v>
       </c>
       <c r="C166" t="s">
+        <v>343</v>
+      </c>
+      <c r="D166" t="s">
         <v>344</v>
-      </c>
-      <c r="D166" t="s">
-        <v>345</v>
       </c>
       <c r="E166" t="s">
         <v>16</v>
@@ -7961,18 +7964,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B167">
         <v>166</v>
       </c>
       <c r="C167" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D167" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E167" t="s">
         <v>29</v>
@@ -7996,18 +7999,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B168">
         <v>167</v>
       </c>
       <c r="C168" t="s">
+        <v>346</v>
+      </c>
+      <c r="D168" t="s">
         <v>347</v>
-      </c>
-      <c r="D168" t="s">
-        <v>348</v>
       </c>
       <c r="E168" t="s">
         <v>106</v>
@@ -8031,18 +8034,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B169">
         <v>168</v>
       </c>
       <c r="C169" t="s">
+        <v>348</v>
+      </c>
+      <c r="D169" t="s">
         <v>349</v>
-      </c>
-      <c r="D169" t="s">
-        <v>350</v>
       </c>
       <c r="E169" t="s">
         <v>29</v>
@@ -8066,18 +8069,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B170">
         <v>169</v>
       </c>
       <c r="C170" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D170" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E170" t="s">
         <v>29</v>
@@ -8101,18 +8104,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B171">
         <v>170</v>
       </c>
       <c r="C171" t="s">
+        <v>351</v>
+      </c>
+      <c r="D171" t="s">
         <v>352</v>
-      </c>
-      <c r="D171" t="s">
-        <v>353</v>
       </c>
       <c r="E171" t="s">
         <v>29</v>
@@ -8136,18 +8139,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B172">
         <v>171</v>
       </c>
       <c r="C172" t="s">
+        <v>353</v>
+      </c>
+      <c r="D172" t="s">
         <v>354</v>
-      </c>
-      <c r="D172" t="s">
-        <v>355</v>
       </c>
       <c r="E172" t="s">
         <v>29</v>
@@ -8174,18 +8177,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B173">
         <v>172</v>
       </c>
       <c r="C173" t="s">
+        <v>355</v>
+      </c>
+      <c r="D173" t="s">
         <v>356</v>
-      </c>
-      <c r="D173" t="s">
-        <v>357</v>
       </c>
       <c r="E173" t="s">
         <v>16</v>
@@ -8221,18 +8224,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B174">
         <v>173</v>
       </c>
       <c r="C174" t="s">
+        <v>357</v>
+      </c>
+      <c r="D174" t="s">
         <v>358</v>
-      </c>
-      <c r="D174" t="s">
-        <v>359</v>
       </c>
       <c r="E174" t="s">
         <v>29</v>
@@ -8268,18 +8271,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B175">
         <v>174</v>
       </c>
       <c r="C175" t="s">
+        <v>359</v>
+      </c>
+      <c r="D175" t="s">
         <v>360</v>
-      </c>
-      <c r="D175" t="s">
-        <v>361</v>
       </c>
       <c r="E175" t="s">
         <v>16</v>
@@ -8303,21 +8306,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B176">
         <v>175</v>
       </c>
       <c r="C176" t="s">
+        <v>361</v>
+      </c>
+      <c r="D176" t="s">
         <v>362</v>
       </c>
-      <c r="D176" t="s">
-        <v>363</v>
-      </c>
       <c r="E176" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F176">
         <v>4</v>
@@ -8338,18 +8341,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B177">
         <v>176</v>
       </c>
       <c r="C177" t="s">
+        <v>363</v>
+      </c>
+      <c r="D177" t="s">
         <v>364</v>
-      </c>
-      <c r="D177" t="s">
-        <v>365</v>
       </c>
       <c r="E177" t="s">
         <v>29</v>
@@ -8373,18 +8376,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B178">
         <v>177</v>
       </c>
       <c r="C178" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D178" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E178" t="s">
         <v>29</v>
@@ -8408,18 +8411,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B179">
         <v>178</v>
       </c>
       <c r="C179" t="s">
+        <v>366</v>
+      </c>
+      <c r="D179" t="s">
         <v>367</v>
-      </c>
-      <c r="D179" t="s">
-        <v>368</v>
       </c>
       <c r="E179" t="s">
         <v>16</v>
@@ -8446,18 +8449,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B180">
         <v>179</v>
       </c>
       <c r="C180" t="s">
+        <v>368</v>
+      </c>
+      <c r="D180" t="s">
         <v>369</v>
-      </c>
-      <c r="D180" t="s">
-        <v>370</v>
       </c>
       <c r="E180" t="s">
         <v>106</v>
@@ -8493,21 +8496,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B181">
         <v>180</v>
       </c>
       <c r="C181" t="s">
+        <v>370</v>
+      </c>
+      <c r="D181" t="s">
         <v>371</v>
       </c>
-      <c r="D181" t="s">
-        <v>372</v>
-      </c>
       <c r="E181" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F181">
         <v>4</v>
@@ -8531,18 +8534,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B182">
         <v>181</v>
       </c>
       <c r="C182" t="s">
+        <v>372</v>
+      </c>
+      <c r="D182" t="s">
         <v>373</v>
-      </c>
-      <c r="D182" t="s">
-        <v>374</v>
       </c>
       <c r="E182" t="s">
         <v>16</v>
@@ -8566,18 +8569,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B183">
         <v>182</v>
       </c>
       <c r="C183" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D183" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E183" t="s">
         <v>29</v>
@@ -8604,18 +8607,18 @@
         <v>24</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B184">
         <v>183</v>
       </c>
       <c r="C184" t="s">
+        <v>375</v>
+      </c>
+      <c r="D184" t="s">
         <v>376</v>
-      </c>
-      <c r="D184" t="s">
-        <v>377</v>
       </c>
       <c r="E184" t="s">
         <v>106</v>

</xml_diff>